<commit_message>
Verification: Adding sealed compartment hand calculation test to guide
</commit_message>
<xml_diff>
--- a/cfast/trunk/Verification/Analytical/sealed_test_hand_calc.xlsx
+++ b/cfast/trunk/Verification/Analytical/sealed_test_hand_calc.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpeacoc\Documents\Visual Studio 2010\Projects\cfast\Verification\Mass_Energy_Balance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpeacoc\Documents\Visual Studio 2010\Projects\cfast\Verification\Analytical\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="840" yWindow="4800" windowWidth="19635" windowHeight="10995"/>
+    <workbookView xWindow="840" yWindow="5400" windowWidth="19635" windowHeight="10995"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -715,274 +715,274 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>402.37799999999999</c:v>
+                  <c:v>3219.29</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>804.76499999999999</c:v>
+                  <c:v>6439.18</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1207.1600000000001</c:v>
+                  <c:v>9659.66</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1609.57</c:v>
+                  <c:v>12880.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2011.98</c:v>
+                  <c:v>16102.4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2414.41</c:v>
+                  <c:v>19324.7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2816.84</c:v>
+                  <c:v>22547.599999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3219.29</c:v>
+                  <c:v>25771.1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3621.74</c:v>
+                  <c:v>28995.200000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4024.2</c:v>
+                  <c:v>32219.9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4426.67</c:v>
+                  <c:v>35445.199999999997</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4829.16</c:v>
+                  <c:v>38671.1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5231.6499999999996</c:v>
+                  <c:v>41897.599999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5634.15</c:v>
+                  <c:v>45124.7</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6036.66</c:v>
+                  <c:v>48352.4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6439.18</c:v>
+                  <c:v>51580.7</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6841.7</c:v>
+                  <c:v>54809.599999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7244.24</c:v>
+                  <c:v>58039.1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7646.79</c:v>
+                  <c:v>61269.1</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>8049.34</c:v>
+                  <c:v>64499.8</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>8451.91</c:v>
+                  <c:v>67731.100000000006</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>8854.49</c:v>
+                  <c:v>70963</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9257.07</c:v>
+                  <c:v>74195.5</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>9659.66</c:v>
+                  <c:v>77428.600000000006</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>10062.299999999999</c:v>
+                  <c:v>80662.3</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>10464.9</c:v>
+                  <c:v>83896.6</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>10867.5</c:v>
+                  <c:v>87131.5</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>11270.1</c:v>
+                  <c:v>90367</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>11672.8</c:v>
+                  <c:v>93603.1</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>12075.4</c:v>
+                  <c:v>96839.8</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>12478.1</c:v>
+                  <c:v>100077</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>12880.8</c:v>
+                  <c:v>103315</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>13283.4</c:v>
+                  <c:v>106553</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>13686.1</c:v>
+                  <c:v>109793</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>14088.8</c:v>
+                  <c:v>113032</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>14491.5</c:v>
+                  <c:v>116272</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>14894.2</c:v>
+                  <c:v>119513</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>15297</c:v>
+                  <c:v>122755</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>15699.7</c:v>
+                  <c:v>125997</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>16102.4</c:v>
+                  <c:v>129240</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>16505.2</c:v>
+                  <c:v>132483</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>16908</c:v>
+                  <c:v>135727</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>17310.7</c:v>
+                  <c:v>138971</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>17713.5</c:v>
+                  <c:v>142216</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>18116.3</c:v>
+                  <c:v>145462</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>18519.099999999999</c:v>
+                  <c:v>148708</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>18921.900000000001</c:v>
+                  <c:v>151955</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>19324.7</c:v>
+                  <c:v>155203</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>19727.599999999999</c:v>
+                  <c:v>158451</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>20130.400000000001</c:v>
+                  <c:v>161699</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>20533.2</c:v>
+                  <c:v>164949</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>20936.099999999999</c:v>
+                  <c:v>168199</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>21339</c:v>
+                  <c:v>171449</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>21741.8</c:v>
+                  <c:v>174700</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>22144.7</c:v>
+                  <c:v>177952</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>22547.599999999999</c:v>
+                  <c:v>181204</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>22950.5</c:v>
+                  <c:v>184457</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>23353.4</c:v>
+                  <c:v>187710</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>23756.400000000001</c:v>
+                  <c:v>190964</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>24159.3</c:v>
+                  <c:v>194219</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>24562.2</c:v>
+                  <c:v>197474</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>24965.200000000001</c:v>
+                  <c:v>200730</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>25368.1</c:v>
+                  <c:v>203987</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>25771.1</c:v>
+                  <c:v>207244</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>26174.1</c:v>
+                  <c:v>210501</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>26577.1</c:v>
+                  <c:v>213759</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>26980.1</c:v>
+                  <c:v>217018</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>27383.1</c:v>
+                  <c:v>220278</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>27786.1</c:v>
+                  <c:v>223538</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>28189.1</c:v>
+                  <c:v>226798</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>28592.2</c:v>
+                  <c:v>230060</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>28995.200000000001</c:v>
+                  <c:v>233321</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>29398.3</c:v>
+                  <c:v>236584</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>29801.3</c:v>
+                  <c:v>239847</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>30204.400000000001</c:v>
+                  <c:v>243111</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>30607.5</c:v>
+                  <c:v>246375</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>31010.6</c:v>
+                  <c:v>249640</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>31413.7</c:v>
+                  <c:v>252905</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>31816.799999999999</c:v>
+                  <c:v>256171</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>32219.9</c:v>
+                  <c:v>259438</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>32623</c:v>
+                  <c:v>262705</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>33026.199999999997</c:v>
+                  <c:v>265973</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>33429.300000000003</c:v>
+                  <c:v>269241</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>33832.5</c:v>
+                  <c:v>272510</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>34235.599999999999</c:v>
+                  <c:v>275780</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>34638.800000000003</c:v>
+                  <c:v>279050</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>35042</c:v>
+                  <c:v>282321</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>35445.199999999997</c:v>
+                  <c:v>285592</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>35848.400000000001</c:v>
+                  <c:v>288864</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>36251.599999999999</c:v>
+                  <c:v>292136</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -997,11 +997,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="223673504"/>
-        <c:axId val="226429744"/>
+        <c:axId val="205504120"/>
+        <c:axId val="205502944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="223673504"/>
+        <c:axId val="205504120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1058,12 +1058,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="226429744"/>
+        <c:crossAx val="205502944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="226429744"/>
+        <c:axId val="205502944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1120,7 +1120,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223673504"/>
+        <c:crossAx val="205504120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1603,274 +1603,274 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.159600000000001</c:v>
+                  <c:v>29.276399999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22.319199999999999</c:v>
+                  <c:v>38.552100000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.4787</c:v>
+                  <c:v>47.827100000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24.638300000000001</c:v>
+                  <c:v>57.101300000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25.797799999999999</c:v>
+                  <c:v>66.374799999999993</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26.9574</c:v>
+                  <c:v>75.647599999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>28.116900000000001</c:v>
+                  <c:v>84.919700000000006</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>29.276399999999999</c:v>
+                  <c:v>94.191000000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>30.4359</c:v>
+                  <c:v>103.462</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>31.595400000000001</c:v>
+                  <c:v>112.73099999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>32.754899999999999</c:v>
+                  <c:v>122.001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>33.914299999999997</c:v>
+                  <c:v>131.26900000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>35.073799999999999</c:v>
+                  <c:v>140.53700000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>36.233199999999997</c:v>
+                  <c:v>149.804</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>37.392699999999998</c:v>
+                  <c:v>159.07</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>38.552100000000003</c:v>
+                  <c:v>168.33500000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>39.711500000000001</c:v>
+                  <c:v>177.6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>40.870899999999999</c:v>
+                  <c:v>186.864</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>42.030299999999997</c:v>
+                  <c:v>196.12799999999999</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>43.189700000000002</c:v>
+                  <c:v>205.39</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44.348999999999997</c:v>
+                  <c:v>214.65199999999999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>45.508400000000002</c:v>
+                  <c:v>223.91300000000001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>46.667700000000004</c:v>
+                  <c:v>233.17400000000001</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>47.827100000000002</c:v>
+                  <c:v>242.43299999999999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>48.986400000000003</c:v>
+                  <c:v>251.69200000000001</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>50.145699999999998</c:v>
+                  <c:v>260.95</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>51.305</c:v>
+                  <c:v>270.20800000000003</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>52.464300000000001</c:v>
+                  <c:v>279.46499999999997</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>53.6235</c:v>
+                  <c:v>288.721</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>54.782800000000002</c:v>
+                  <c:v>297.976</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>55.942100000000003</c:v>
+                  <c:v>307.23099999999999</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>57.101300000000002</c:v>
+                  <c:v>316.48399999999998</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>58.2605</c:v>
+                  <c:v>325.73700000000002</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>59.419699999999999</c:v>
+                  <c:v>334.99</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>60.579000000000001</c:v>
+                  <c:v>344.24099999999999</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>61.738100000000003</c:v>
+                  <c:v>353.49200000000002</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>62.897300000000001</c:v>
+                  <c:v>362.74299999999999</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>64.0565</c:v>
+                  <c:v>371.99200000000002</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>65.215699999999998</c:v>
+                  <c:v>381.24099999999999</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>66.374799999999993</c:v>
+                  <c:v>390.48899999999998</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>67.533900000000003</c:v>
+                  <c:v>399.73599999999999</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>68.693100000000001</c:v>
+                  <c:v>408.983</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>69.852199999999996</c:v>
+                  <c:v>418.22800000000001</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>71.011300000000006</c:v>
+                  <c:v>427.47300000000001</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>72.170400000000001</c:v>
+                  <c:v>436.71800000000002</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>73.329499999999996</c:v>
+                  <c:v>445.96100000000001</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>74.488500000000002</c:v>
+                  <c:v>455.20400000000001</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>75.647599999999997</c:v>
+                  <c:v>464.44600000000003</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>76.806600000000003</c:v>
+                  <c:v>473.68799999999999</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>77.965699999999998</c:v>
+                  <c:v>482.92899999999997</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>79.124700000000004</c:v>
+                  <c:v>492.16899999999998</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>80.283699999999996</c:v>
+                  <c:v>501.40800000000002</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>81.442700000000002</c:v>
+                  <c:v>510.64600000000002</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>82.601699999999994</c:v>
+                  <c:v>519.88400000000001</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>83.7607</c:v>
+                  <c:v>529.12099999999998</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>84.919700000000006</c:v>
+                  <c:v>538.35799999999995</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>86.078599999999994</c:v>
+                  <c:v>547.59299999999996</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>87.2376</c:v>
+                  <c:v>556.82799999999997</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>88.396500000000003</c:v>
+                  <c:v>566.06200000000001</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>89.555400000000006</c:v>
+                  <c:v>575.29600000000005</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>90.714299999999994</c:v>
+                  <c:v>584.52800000000002</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>91.873199999999997</c:v>
+                  <c:v>593.76</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>93.0321</c:v>
+                  <c:v>602.99099999999999</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>94.191000000000003</c:v>
+                  <c:v>612.22199999999998</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>95.349900000000005</c:v>
+                  <c:v>621.452</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>96.508700000000005</c:v>
+                  <c:v>630.68100000000004</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>97.667500000000004</c:v>
+                  <c:v>639.90899999999999</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>98.826400000000007</c:v>
+                  <c:v>649.13699999999994</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>99.985200000000006</c:v>
+                  <c:v>658.36300000000006</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>101.14400000000001</c:v>
+                  <c:v>667.59</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>102.303</c:v>
+                  <c:v>676.81500000000005</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>103.462</c:v>
+                  <c:v>686.04</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>104.62</c:v>
+                  <c:v>695.26400000000001</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>105.779</c:v>
+                  <c:v>704.48699999999997</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>106.938</c:v>
+                  <c:v>713.70899999999995</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>108.09699999999999</c:v>
+                  <c:v>722.93100000000004</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>109.255</c:v>
+                  <c:v>732.15200000000004</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>110.414</c:v>
+                  <c:v>741.37199999999996</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>111.57299999999999</c:v>
+                  <c:v>750.59199999999998</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>112.73099999999999</c:v>
+                  <c:v>759.81100000000004</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>113.89</c:v>
+                  <c:v>769.029</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>115.04900000000001</c:v>
+                  <c:v>778.24599999999998</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>116.20699999999999</c:v>
+                  <c:v>787.46299999999997</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>117.366</c:v>
+                  <c:v>796.67899999999997</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>118.52500000000001</c:v>
+                  <c:v>805.89400000000001</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>119.68300000000001</c:v>
+                  <c:v>815.10900000000004</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>120.842</c:v>
+                  <c:v>824.322</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>122.001</c:v>
+                  <c:v>833.53499999999997</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>123.15900000000001</c:v>
+                  <c:v>842.74800000000005</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>124.318</c:v>
+                  <c:v>851.95899999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1885,11 +1885,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="226434056"/>
-        <c:axId val="226432880"/>
+        <c:axId val="309248104"/>
+        <c:axId val="309247712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="226434056"/>
+        <c:axId val="309248104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1946,12 +1946,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="226432880"/>
+        <c:crossAx val="309247712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="226432880"/>
+        <c:axId val="309247712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2008,7 +2008,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="226434056"/>
+        <c:crossAx val="309248104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3524,7 +3524,7 @@
   <dimension ref="A1:R101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="K11" sqref="K11:K101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3816,27 +3816,27 @@
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="2">
-        <v>21.159600000000001</v>
+        <v>29.276399999999999</v>
       </c>
       <c r="H12" s="4">
         <f t="shared" si="1"/>
-        <v>-8.1161990216007887</v>
+        <v>6.0097839920913998E-4</v>
       </c>
       <c r="I12" s="9">
         <f>H12/(E12+273.15)*100</f>
-        <v>-2.6836992901591339</v>
+        <v>1.9871928954256151E-4</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2">
-        <v>402.37799999999999</v>
+        <v>3219.29</v>
       </c>
       <c r="L12" s="4">
         <f t="shared" si="2"/>
-        <v>-2797.6219999999994</v>
+        <v>19.290000000000418</v>
       </c>
       <c r="M12" s="9">
         <f t="shared" si="3"/>
-        <v>-2.6771502392344493</v>
+        <v>1.8459330143541067E-2</v>
       </c>
       <c r="O12" s="3" t="s">
         <v>31</v>
@@ -3868,27 +3868,27 @@
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="2">
-        <v>22.319199999999999</v>
+        <v>38.552100000000003</v>
       </c>
       <c r="H13" s="4">
         <f t="shared" si="1"/>
-        <v>-16.233391345340717</v>
+        <v>-4.9134534071271219E-4</v>
       </c>
       <c r="I13" s="9">
         <f t="shared" ref="I13:I76" si="8">H13/(E13+273.15)*100</f>
-        <v>-5.2079744590109813</v>
+        <v>-1.5763274170805408E-4</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2">
-        <v>804.76499999999999</v>
+        <v>6439.18</v>
       </c>
       <c r="L13" s="4">
         <f t="shared" si="2"/>
-        <v>-5595.2349999999988</v>
+        <v>39.180000000001201</v>
       </c>
       <c r="M13" s="9">
         <f t="shared" si="3"/>
-        <v>-5.1952042711234903</v>
+        <v>3.6378830083566578E-2</v>
       </c>
       <c r="O13" s="3" t="s">
         <v>37</v>
@@ -3920,27 +3920,27 @@
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="2">
-        <v>23.4787</v>
+        <v>47.827100000000002</v>
       </c>
       <c r="H14" s="4">
         <f t="shared" si="1"/>
-        <v>-24.351677130750833</v>
+        <v>-3.2771307508312475E-3</v>
       </c>
       <c r="I14" s="9">
         <f t="shared" si="8"/>
-        <v>-7.5866560281444295</v>
+        <v>-1.0209754191597557E-3</v>
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2">
-        <v>1207.1600000000001</v>
+        <v>9659.66</v>
       </c>
       <c r="L14" s="4">
         <f t="shared" si="2"/>
-        <v>-8392.8399999999983</v>
+        <v>59.660000000001673</v>
       </c>
       <c r="M14" s="9">
         <f t="shared" si="3"/>
-        <v>-7.5679350766456253</v>
+        <v>5.3796212804329731E-2</v>
       </c>
       <c r="O14" s="3" t="s">
         <v>33</v>
@@ -3972,27 +3972,27 @@
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="2">
-        <v>24.638300000000001</v>
+        <v>57.101300000000002</v>
       </c>
       <c r="H15" s="4">
         <f t="shared" si="1"/>
-        <v>-32.470856537395903</v>
+        <v>-7.8565373959023077E-3</v>
       </c>
       <c r="I15" s="9">
         <f t="shared" si="8"/>
-        <v>-9.8319322552133901</v>
+        <v>-2.3789007027917777E-3</v>
       </c>
       <c r="J15" s="2"/>
       <c r="K15" s="2">
-        <v>1609.57</v>
+        <v>12880.8</v>
       </c>
       <c r="L15" s="4">
         <f t="shared" si="2"/>
-        <v>-11190.429999999998</v>
+        <v>80.800000000001091</v>
       </c>
       <c r="M15" s="9">
         <f t="shared" si="3"/>
-        <v>-9.8075635407537227</v>
+        <v>7.0815074496057048E-2</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -4018,27 +4018,27 @@
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="2">
-        <v>25.797799999999999</v>
+        <v>66.374799999999993</v>
       </c>
       <c r="H16" s="4">
         <f t="shared" si="1"/>
-        <v>-40.591129724875145</v>
+        <v>-1.4129724875147076E-2</v>
       </c>
       <c r="I16" s="9">
         <f t="shared" si="8"/>
-        <v>-11.954779311393164</v>
+        <v>-4.1614447234655082E-3</v>
       </c>
       <c r="J16" s="2"/>
       <c r="K16" s="2">
-        <v>2011.98</v>
+        <v>16102.4</v>
       </c>
       <c r="L16" s="4">
         <f t="shared" si="2"/>
-        <v>-13988.019999999997</v>
+        <v>102.40000000000327</v>
       </c>
       <c r="M16" s="9">
         <f t="shared" si="3"/>
-        <v>-11.924995737425402</v>
+        <v>8.7297527706737654E-2</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -4064,27 +4064,27 @@
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="2">
-        <v>26.9574</v>
+        <v>75.647599999999997</v>
       </c>
       <c r="H17" s="4">
         <f t="shared" si="1"/>
-        <v>-48.712296852821858</v>
+        <v>-2.209685282186058E-2</v>
       </c>
       <c r="I17" s="9">
         <f t="shared" si="8"/>
-        <v>-13.964892834986648</v>
+        <v>-6.3347491615944919E-3</v>
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2">
-        <v>2414.41</v>
+        <v>19324.7</v>
       </c>
       <c r="L17" s="4">
         <f t="shared" si="2"/>
-        <v>-16785.589999999997</v>
+        <v>124.70000000000437</v>
       </c>
       <c r="M17" s="9">
         <f t="shared" si="3"/>
-        <v>-13.929950207468877</v>
+        <v>0.10348547717842686</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -4110,27 +4110,27 @@
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="2">
-        <v>28.116900000000001</v>
+        <v>84.919700000000006</v>
       </c>
       <c r="H18" s="4">
         <f t="shared" si="1"/>
-        <v>-56.83455808090342</v>
+        <v>-3.1758080903415475E-2</v>
       </c>
       <c r="I18" s="9">
         <f t="shared" si="8"/>
-        <v>-15.871076980664842</v>
+        <v>-8.8684589762939737E-3</v>
       </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2">
-        <v>2816.84</v>
+        <v>22547.599999999999</v>
       </c>
       <c r="L18" s="4">
         <f t="shared" si="2"/>
-        <v>-19583.159999999996</v>
+        <v>147.60000000000218</v>
       </c>
       <c r="M18" s="9">
         <f t="shared" si="3"/>
-        <v>-15.831172190784152</v>
+        <v>0.11932093775262909</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -4156,27 +4156,27 @@
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="2">
-        <v>29.276399999999999</v>
+        <v>94.191000000000003</v>
       </c>
       <c r="H19" s="4">
         <f t="shared" si="1"/>
-        <v>-64.957813568821592</v>
+        <v>-4.3213568821585113E-2</v>
       </c>
       <c r="I19" s="9">
         <f t="shared" si="8"/>
-        <v>-17.681166247676327</v>
+        <v>-1.1762500190686604E-2</v>
       </c>
       <c r="J19" s="2"/>
       <c r="K19" s="2">
-        <v>3219.29</v>
+        <v>25771.1</v>
       </c>
       <c r="L19" s="4">
         <f t="shared" si="2"/>
-        <v>-22380.709999999995</v>
+        <v>171.10000000000218</v>
       </c>
       <c r="M19" s="9">
         <f t="shared" si="3"/>
-        <v>-17.636493301812447</v>
+        <v>0.13483057525610889</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -4202,27 +4202,27 @@
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="2">
-        <v>30.4359</v>
+        <v>103.462</v>
       </c>
       <c r="H20" s="4">
         <f t="shared" si="1"/>
-        <v>-73.082063476312271</v>
+        <v>-5.5963476312271609E-2</v>
       </c>
       <c r="I20" s="9">
         <f t="shared" si="8"/>
-        <v>-19.402250937889555</v>
+        <v>-1.4857508930618416E-2</v>
       </c>
       <c r="J20" s="2"/>
       <c r="K20" s="2">
-        <v>3621.74</v>
+        <v>28995.200000000001</v>
       </c>
       <c r="L20" s="4">
         <f t="shared" si="2"/>
-        <v>-25178.259999999995</v>
+        <v>195.20000000000437</v>
       </c>
       <c r="M20" s="9">
         <f t="shared" si="3"/>
-        <v>-19.353005380476553</v>
+        <v>0.15003843197540689</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -4248,27 +4248,27 @@
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="2">
-        <v>31.595400000000001</v>
+        <v>112.73099999999999</v>
       </c>
       <c r="H21" s="4">
         <f t="shared" si="1"/>
-        <v>-81.207307963145567</v>
+        <v>-7.1707963145570375E-2</v>
       </c>
       <c r="I21" s="9">
         <f t="shared" si="8"/>
-        <v>-21.040740559047979</v>
+        <v>-1.8579468848400393E-2</v>
       </c>
       <c r="J21" s="2"/>
       <c r="K21" s="2">
-        <v>4024.2</v>
+        <v>32219.9</v>
       </c>
       <c r="L21" s="4">
         <f t="shared" si="2"/>
-        <v>-27975.799999999992</v>
+        <v>219.90000000000873</v>
       </c>
       <c r="M21" s="9">
         <f t="shared" si="3"/>
-        <v>-20.987096774193542</v>
+        <v>0.16496624156039666</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -4294,27 +4294,27 @@
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="2">
-        <v>32.754899999999999</v>
+        <v>122.001</v>
       </c>
       <c r="H22" s="4">
         <f t="shared" si="1"/>
-        <v>-89.33354718912571</v>
+        <v>-8.7447189125697378E-2</v>
       </c>
       <c r="I22" s="9">
         <f t="shared" si="8"/>
-        <v>-22.602443619655929</v>
+        <v>-2.2125172727402453E-2</v>
       </c>
       <c r="J22" s="2"/>
       <c r="K22" s="2">
-        <v>4426.67</v>
+        <v>35445.199999999997</v>
       </c>
       <c r="L22" s="4">
         <f t="shared" si="2"/>
-        <v>-30773.329999999994</v>
+        <v>245.20000000000437</v>
       </c>
       <c r="M22" s="9">
         <f t="shared" si="3"/>
-        <v>-22.544564102564099</v>
+        <v>0.17963369963370282</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -4340,27 +4340,27 @@
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="2">
-        <v>33.914299999999997</v>
+        <v>131.26900000000001</v>
       </c>
       <c r="H23" s="4">
         <f t="shared" si="1"/>
-        <v>-97.460881314091324</v>
+        <v>-0.10618131409131593</v>
       </c>
       <c r="I23" s="9">
         <f t="shared" si="8"/>
-        <v>-24.092661178098172</v>
+        <v>-2.624838180564884E-2</v>
       </c>
       <c r="J23" s="2"/>
       <c r="K23" s="2">
-        <v>4829.16</v>
+        <v>38671.1</v>
       </c>
       <c r="L23" s="4">
         <f t="shared" si="2"/>
-        <v>-33570.839999999997</v>
+        <v>271.10000000000582</v>
       </c>
       <c r="M23" s="9">
         <f t="shared" si="3"/>
-        <v>-24.030665712240513</v>
+        <v>0.19405869720830768</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -4386,27 +4386,27 @@
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="2">
-        <v>35.073799999999999</v>
+        <v>140.53700000000001</v>
       </c>
       <c r="H24" s="4">
         <f t="shared" si="1"/>
-        <v>-105.58911049791504</v>
+        <v>-0.12591049791504361</v>
       </c>
       <c r="I24" s="9">
         <f t="shared" si="8"/>
-        <v>-25.516146987986986</v>
+        <v>-3.0426913883267546E-2</v>
       </c>
       <c r="J24" s="2"/>
       <c r="K24" s="2">
-        <v>5231.6499999999996</v>
+        <v>41897.599999999999</v>
       </c>
       <c r="L24" s="4">
         <f t="shared" si="2"/>
-        <v>-36368.349999999991</v>
+        <v>297.60000000000582</v>
       </c>
       <c r="M24" s="9">
         <f t="shared" si="3"/>
-        <v>-25.450209937018887</v>
+        <v>0.20825752274318113</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -4432,27 +4432,27 @@
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="2">
-        <v>36.233199999999997</v>
+        <v>149.804</v>
       </c>
       <c r="H25" s="4">
         <f t="shared" si="1"/>
-        <v>-113.71843490050419</v>
+        <v>-0.14763490050418682</v>
       </c>
       <c r="I25" s="9">
         <f t="shared" si="8"/>
-        <v>-26.877332895970969</v>
+        <v>-3.4893483817169453E-2</v>
       </c>
       <c r="J25" s="2"/>
       <c r="K25" s="2">
-        <v>5634.15</v>
+        <v>45124.7</v>
       </c>
       <c r="L25" s="4">
         <f t="shared" si="2"/>
-        <v>-39165.849999999991</v>
+        <v>324.70000000000437</v>
       </c>
       <c r="M25" s="9">
         <f t="shared" si="3"/>
-        <v>-26.807563312799449</v>
+        <v>0.22224503764545128</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -4478,27 +4478,27 @@
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="2">
-        <v>37.392699999999998</v>
+        <v>159.07</v>
       </c>
       <c r="H26" s="4">
         <f t="shared" si="1"/>
-        <v>-121.84865468179987</v>
+        <v>-0.17135468179986901</v>
       </c>
       <c r="I26" s="9">
         <f t="shared" si="8"/>
-        <v>-28.180178295070039</v>
+        <v>-3.9629534666799769E-2</v>
       </c>
       <c r="J26" s="2"/>
       <c r="K26" s="2">
-        <v>6036.66</v>
+        <v>48352.4</v>
       </c>
       <c r="L26" s="4">
         <f t="shared" si="2"/>
-        <v>-41963.34</v>
+        <v>352.40000000000873</v>
       </c>
       <c r="M26" s="9">
         <f t="shared" si="3"/>
-        <v>-28.106724715338245</v>
+        <v>0.23603482920295293</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -4524,27 +4524,27 @@
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="2">
-        <v>38.552100000000003</v>
+        <v>168.33500000000001</v>
       </c>
       <c r="H27" s="4">
         <f t="shared" si="1"/>
-        <v>-129.97997000177764</v>
+        <v>-0.19707000177763234</v>
       </c>
       <c r="I27" s="9">
         <f t="shared" si="8"/>
-        <v>-29.428400840734721</v>
+        <v>-4.4618066967680892E-2</v>
       </c>
       <c r="J27" s="2"/>
       <c r="K27" s="2">
-        <v>6439.18</v>
+        <v>51580.7</v>
       </c>
       <c r="L27" s="4">
         <f t="shared" si="2"/>
-        <v>-44760.819999999992</v>
+        <v>380.70000000000437</v>
       </c>
       <c r="M27" s="9">
         <f t="shared" si="3"/>
-        <v>-29.351357377049176</v>
+        <v>0.24963934426229795</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -4570,27 +4570,27 @@
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="2">
-        <v>39.711500000000001</v>
+        <v>177.6</v>
       </c>
       <c r="H28" s="4">
         <f t="shared" si="1"/>
-        <v>-138.11228102044743</v>
+        <v>-0.22378102044743287</v>
       </c>
       <c r="I28" s="9">
         <f t="shared" si="8"/>
-        <v>-30.625346047375938</v>
+        <v>-4.9621736310494401E-2</v>
       </c>
       <c r="J28" s="2"/>
       <c r="K28" s="2">
-        <v>6841.7</v>
+        <v>54809.599999999999</v>
       </c>
       <c r="L28" s="4">
         <f t="shared" si="2"/>
-        <v>-47558.299999999996</v>
+        <v>409.60000000000582</v>
       </c>
       <c r="M28" s="9">
         <f t="shared" si="3"/>
-        <v>-30.544829800899166</v>
+        <v>0.2630700064226113</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -4616,27 +4616,27 @@
       </c>
       <c r="F29" s="4"/>
       <c r="G29" s="2">
-        <v>40.870899999999999</v>
+        <v>186.864</v>
       </c>
       <c r="H29" s="4">
         <f t="shared" si="1"/>
-        <v>-146.24558789785323</v>
+        <v>-0.25248789785322856</v>
       </c>
       <c r="I29" s="9">
         <f t="shared" si="8"/>
-        <v>-31.774111681645927</v>
+        <v>-5.4856893667492711E-2</v>
       </c>
       <c r="J29" s="2"/>
       <c r="K29" s="2">
-        <v>7244.24</v>
+        <v>58039.1</v>
       </c>
       <c r="L29" s="4">
         <f t="shared" si="2"/>
-        <v>-50355.759999999995</v>
+        <v>439.10000000000582</v>
       </c>
       <c r="M29" s="9">
         <f t="shared" si="3"/>
-        <v>-31.690220264317176</v>
+        <v>0.27633731906860026</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -4662,27 +4662,27 @@
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="2">
-        <v>42.030299999999997</v>
+        <v>196.12799999999999</v>
       </c>
       <c r="H30" s="4">
         <f t="shared" si="1"/>
-        <v>-154.3798907940735</v>
+        <v>-0.28219079407352865</v>
       </c>
       <c r="I30" s="9">
         <f t="shared" si="8"/>
-        <v>-32.877550912695895</v>
+        <v>-6.0096830950748963E-2</v>
       </c>
       <c r="J30" s="2"/>
       <c r="K30" s="2">
-        <v>7646.79</v>
+        <v>61269.1</v>
       </c>
       <c r="L30" s="4">
         <f t="shared" si="2"/>
-        <v>-53153.209999999992</v>
+        <v>469.10000000000582</v>
       </c>
       <c r="M30" s="9">
         <f t="shared" si="3"/>
-        <v>-32.790382479950644</v>
+        <v>0.28938926588525959</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -4708,27 +4708,27 @@
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="2">
-        <v>43.189700000000002</v>
+        <v>205.39</v>
       </c>
       <c r="H31" s="4">
         <f t="shared" si="1"/>
-        <v>-162.5151898692211</v>
+        <v>-0.31488986922113327</v>
       </c>
       <c r="I31" s="9">
         <f t="shared" si="8"/>
-        <v>-33.938295986411504</v>
+        <v>-6.5758933631675356E-2</v>
       </c>
       <c r="J31" s="2"/>
       <c r="K31" s="2">
-        <v>8049.34</v>
+        <v>64499.8</v>
       </c>
       <c r="L31" s="4">
         <f t="shared" si="2"/>
-        <v>-55950.659999999989</v>
+        <v>499.80000000001746</v>
       </c>
       <c r="M31" s="9">
         <f t="shared" si="3"/>
-        <v>-33.847949183303079</v>
+        <v>0.30235934664247877</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -4754,27 +4754,27 @@
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="2">
-        <v>44.348999999999997</v>
+        <v>214.65199999999999</v>
       </c>
       <c r="H32" s="4">
         <f t="shared" si="1"/>
-        <v>-170.65158528344301</v>
+        <v>-0.34858528344301476</v>
       </c>
       <c r="I32" s="9">
         <f t="shared" si="8"/>
-        <v>-34.958799687673171</v>
+        <v>-7.140937529361148E-2</v>
       </c>
       <c r="J32" s="2"/>
       <c r="K32" s="2">
-        <v>8451.91</v>
+        <v>67731.100000000006</v>
       </c>
       <c r="L32" s="4">
         <f t="shared" si="2"/>
-        <v>-58748.089999999982</v>
+        <v>531.10000000002037</v>
       </c>
       <c r="M32" s="9">
         <f t="shared" si="3"/>
-        <v>-34.865335311572686</v>
+        <v>0.31519287833829102</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -4800,27 +4800,27 @@
       </c>
       <c r="F33" s="4"/>
       <c r="G33" s="2">
-        <v>45.508400000000002</v>
+        <v>223.91300000000001</v>
       </c>
       <c r="H33" s="4">
         <f t="shared" si="1"/>
-        <v>-178.78887719692051</v>
+        <v>-0.38427719692049322</v>
       </c>
       <c r="I33" s="9">
         <f t="shared" si="8"/>
-        <v>-35.941271646792991</v>
+        <v>-7.724983421074641E-2</v>
       </c>
       <c r="J33" s="2"/>
       <c r="K33" s="2">
-        <v>8854.49</v>
+        <v>70963</v>
       </c>
       <c r="L33" s="4">
         <f t="shared" si="2"/>
-        <v>-61545.509999999987</v>
+        <v>563.00000000001455</v>
       </c>
       <c r="M33" s="9">
         <f t="shared" si="3"/>
-        <v>-35.844793244030278</v>
+        <v>0.32789749563192461</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -4846,27 +4846,27 @@
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="2">
-        <v>46.667700000000004</v>
+        <v>233.17400000000001</v>
       </c>
       <c r="H34" s="4">
         <f t="shared" si="1"/>
-        <v>-186.92726576986931</v>
+        <v>-0.4209657698692979</v>
       </c>
       <c r="I34" s="9">
         <f t="shared" si="8"/>
-        <v>-36.887838734792595</v>
+        <v>-8.3072511481144792E-2</v>
       </c>
       <c r="J34" s="2"/>
       <c r="K34" s="2">
-        <v>9257.07</v>
+        <v>74195.5</v>
       </c>
       <c r="L34" s="4">
         <f t="shared" si="2"/>
-        <v>-64342.929999999986</v>
+        <v>595.50000000001455</v>
       </c>
       <c r="M34" s="9">
         <f t="shared" si="3"/>
-        <v>-36.788410520297305</v>
+        <v>0.34048027444254692</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -4892,27 +4892,27 @@
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="2">
-        <v>47.827100000000002</v>
+        <v>242.43299999999999</v>
       </c>
       <c r="H35" s="4">
         <f t="shared" si="1"/>
-        <v>-195.06655116253953</v>
+        <v>-0.4606511625395342</v>
       </c>
       <c r="I35" s="9">
         <f t="shared" si="8"/>
-        <v>-37.800397451474304</v>
+        <v>-8.9265929636336477E-2</v>
       </c>
       <c r="J35" s="2"/>
       <c r="K35" s="2">
-        <v>9659.66</v>
+        <v>77428.600000000006</v>
       </c>
       <c r="L35" s="4">
         <f t="shared" si="2"/>
-        <v>-67140.339999999982</v>
+        <v>628.60000000002037</v>
       </c>
       <c r="M35" s="9">
         <f t="shared" si="3"/>
-        <v>-37.698113419427273</v>
+        <v>0.35294778214487388</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -4938,27 +4938,27 @@
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="2">
-        <v>48.986400000000003</v>
+        <v>251.69200000000001</v>
       </c>
       <c r="H36" s="4">
         <f t="shared" si="1"/>
-        <v>-203.2069335352154</v>
+        <v>-0.50133353521539448</v>
       </c>
       <c r="I36" s="9">
         <f t="shared" si="8"/>
-        <v>-38.680786556815384</v>
+        <v>-9.5429693918784364E-2</v>
       </c>
       <c r="J36" s="2"/>
       <c r="K36" s="2">
-        <v>10062.299999999999</v>
+        <v>80662.3</v>
       </c>
       <c r="L36" s="4">
         <f t="shared" si="2"/>
-        <v>-69937.699999999983</v>
+        <v>662.30000000001746</v>
       </c>
       <c r="M36" s="9">
         <f t="shared" si="3"/>
-        <v>-38.575675675675662</v>
+        <v>0.36530612244898925</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -4984,27 +4984,27 @@
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="2">
-        <v>50.145699999999998</v>
+        <v>260.95</v>
       </c>
       <c r="H37" s="4">
         <f t="shared" si="1"/>
-        <v>-211.34831304821583</v>
+        <v>-0.54401304821584517</v>
       </c>
       <c r="I37" s="9">
         <f t="shared" si="8"/>
-        <v>-39.530661129680652</v>
+        <v>-0.10175238755863231</v>
       </c>
       <c r="J37" s="2"/>
       <c r="K37" s="2">
-        <v>10464.9</v>
+        <v>83896.6</v>
       </c>
       <c r="L37" s="4">
         <f t="shared" si="2"/>
-        <v>-72735.099999999991</v>
+        <v>696.60000000002037</v>
       </c>
       <c r="M37" s="9">
         <f t="shared" si="3"/>
-        <v>-39.422818428184279</v>
+        <v>0.37756097560976715</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -5030,27 +5030,27 @@
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="2">
-        <v>51.305</v>
+        <v>270.20800000000003</v>
       </c>
       <c r="H38" s="4">
         <f t="shared" si="1"/>
-        <v>-219.49068986189383</v>
+        <v>-0.58768986189380712</v>
       </c>
       <c r="I38" s="9">
         <f t="shared" si="8"/>
-        <v>-40.351581776044931</v>
+        <v>-0.10804201096676028</v>
       </c>
       <c r="J38" s="2"/>
       <c r="K38" s="2">
-        <v>10867.5</v>
+        <v>87131.5</v>
       </c>
       <c r="L38" s="4">
         <f t="shared" si="2"/>
-        <v>-75532.499999999985</v>
+        <v>731.50000000001455</v>
       </c>
       <c r="M38" s="9">
         <f t="shared" si="3"/>
-        <v>-40.241076185402228</v>
+        <v>0.38971763452318303</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -5076,27 +5076,27 @@
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="2">
-        <v>52.464300000000001</v>
+        <v>279.46499999999997</v>
       </c>
       <c r="H39" s="4">
         <f t="shared" si="1"/>
-        <v>-227.63406413663697</v>
+        <v>-0.63336413663699886</v>
       </c>
       <c r="I39" s="9">
         <f t="shared" si="8"/>
-        <v>-41.145004466821646</v>
+        <v>-0.11448097774773998</v>
       </c>
       <c r="J39" s="2"/>
       <c r="K39" s="2">
-        <v>11270.1</v>
+        <v>90367</v>
       </c>
       <c r="L39" s="4">
         <f t="shared" si="2"/>
-        <v>-78329.89999999998</v>
+        <v>767.00000000001455</v>
       </c>
       <c r="M39" s="9">
         <f t="shared" si="3"/>
-        <v>-41.031901519119948</v>
+        <v>0.40178103719225483</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -5122,27 +5122,27 @@
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="2">
-        <v>53.6235</v>
+        <v>288.721</v>
       </c>
       <c r="H40" s="4">
         <f t="shared" si="1"/>
-        <v>-235.77853603286715</v>
+        <v>-0.68103603286715497</v>
       </c>
       <c r="I40" s="9">
         <f t="shared" si="8"/>
-        <v>-41.912306938853881</v>
+        <v>-0.1210618732570662</v>
       </c>
       <c r="J40" s="2"/>
       <c r="K40" s="2">
-        <v>11672.8</v>
+        <v>93603.1</v>
       </c>
       <c r="L40" s="4">
         <f t="shared" si="2"/>
-        <v>-81127.199999999983</v>
+        <v>803.10000000002037</v>
       </c>
       <c r="M40" s="9">
         <f t="shared" si="3"/>
-        <v>-41.796599690880981</v>
+        <v>0.41375579598146334</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -5168,27 +5168,27 @@
       </c>
       <c r="F41" s="4"/>
       <c r="G41" s="2">
-        <v>54.782800000000002</v>
+        <v>297.976</v>
       </c>
       <c r="H41" s="4">
         <f t="shared" si="1"/>
-        <v>-243.92390571104039</v>
+        <v>-0.73070571104040027</v>
       </c>
       <c r="I41" s="9">
         <f t="shared" si="8"/>
-        <v>-42.654725086723964</v>
+        <v>-0.12777776385989018</v>
       </c>
       <c r="J41" s="2"/>
       <c r="K41" s="2">
-        <v>12075.4</v>
+        <v>96839.8</v>
       </c>
       <c r="L41" s="4">
         <f t="shared" si="2"/>
-        <v>-83924.599999999991</v>
+        <v>839.80000000001746</v>
       </c>
       <c r="M41" s="9">
         <f t="shared" si="3"/>
-        <v>-42.536543335022806</v>
+        <v>0.42564622402433727</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
@@ -5214,27 +5214,27 @@
       </c>
       <c r="F42" s="4"/>
       <c r="G42" s="2">
-        <v>55.942100000000003</v>
+        <v>307.23099999999999</v>
       </c>
       <c r="H42" s="4">
         <f t="shared" si="1"/>
-        <v>-252.0702733316476</v>
+        <v>-0.78137333164761458</v>
       </c>
       <c r="I42" s="9">
         <f t="shared" si="8"/>
-        <v>-43.373467536550329</v>
+        <v>-0.13445008959685592</v>
       </c>
       <c r="J42" s="2"/>
       <c r="K42" s="2">
-        <v>12478.1</v>
+        <v>100077</v>
       </c>
       <c r="L42" s="4">
         <f t="shared" si="2"/>
-        <v>-86721.89999999998</v>
+        <v>877.00000000001455</v>
       </c>
       <c r="M42" s="9">
         <f t="shared" si="3"/>
-        <v>-43.252817955112214</v>
+        <v>0.43740648379053099</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -5260,27 +5260,27 @@
       </c>
       <c r="F43" s="4"/>
       <c r="G43" s="2">
-        <v>57.101300000000002</v>
+        <v>316.48399999999998</v>
       </c>
       <c r="H43" s="4">
         <f t="shared" ref="H43:H74" si="10">G43-E43</f>
-        <v>-260.21773905521394</v>
+        <v>-0.83503905521394017</v>
       </c>
       <c r="I43" s="9">
         <f t="shared" si="8"/>
-        <v>-44.069666967056911</v>
+        <v>-0.14141961728426153</v>
       </c>
       <c r="J43" s="2"/>
       <c r="K43" s="2">
-        <v>12880.8</v>
+        <v>103315</v>
       </c>
       <c r="L43" s="4">
         <f t="shared" ref="L43:L74" si="11">K43-C43</f>
-        <v>-89519.199999999983</v>
+        <v>915.00000000001455</v>
       </c>
       <c r="M43" s="9">
         <f t="shared" ref="M43:M74" si="12">L43/(C43+P0)*100</f>
-        <v>-43.946588119783989</v>
+        <v>0.44918998527246667</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -5306,27 +5306,27 @@
       </c>
       <c r="F44" s="4"/>
       <c r="G44" s="2">
-        <v>58.2605</v>
+        <v>325.73700000000002</v>
       </c>
       <c r="H44" s="4">
         <f t="shared" si="10"/>
-        <v>-268.36620304229882</v>
+        <v>-0.88970304229877684</v>
       </c>
       <c r="I44" s="9">
         <f t="shared" si="8"/>
-        <v>-44.744352636746633</v>
+        <v>-0.14833904647944141</v>
       </c>
       <c r="J44" s="2"/>
       <c r="K44" s="2">
-        <v>13283.4</v>
+        <v>106553</v>
       </c>
       <c r="L44" s="4">
         <f t="shared" si="11"/>
-        <v>-92316.599999999991</v>
+        <v>953.00000000001455</v>
       </c>
       <c r="M44" s="9">
         <f t="shared" si="12"/>
-        <v>-44.618946350894149</v>
+        <v>0.46060898985017618</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
@@ -5352,27 +5352,27 @@
       </c>
       <c r="F45" s="4"/>
       <c r="G45" s="2">
-        <v>59.419699999999999</v>
+        <v>334.99</v>
       </c>
       <c r="H45" s="4">
         <f t="shared" si="10"/>
-        <v>-276.51566545349607</v>
+        <v>-0.94536545349603784</v>
       </c>
       <c r="I45" s="9">
         <f t="shared" si="8"/>
-        <v>-45.398507522441562</v>
+        <v>-0.15521066620803861</v>
       </c>
       <c r="J45" s="2"/>
       <c r="K45" s="2">
-        <v>13686.1</v>
+        <v>109793</v>
       </c>
       <c r="L45" s="4">
         <f t="shared" si="11"/>
-        <v>-95113.89999999998</v>
+        <v>993.00000000001455</v>
       </c>
       <c r="M45" s="9">
         <f t="shared" si="12"/>
-        <v>-45.270775821037589</v>
+        <v>0.4726320799619298</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
@@ -5398,27 +5398,27 @@
       </c>
       <c r="F46" s="4"/>
       <c r="G46" s="2">
-        <v>60.579000000000001</v>
+        <v>344.24099999999999</v>
       </c>
       <c r="H46" s="4">
         <f t="shared" si="10"/>
-        <v>-284.66602644943413</v>
+        <v>-1.00402644943415</v>
       </c>
       <c r="I46" s="9">
         <f t="shared" si="8"/>
-        <v>-46.033039444684334</v>
+        <v>-0.16236004600471166</v>
       </c>
       <c r="J46" s="2"/>
       <c r="K46" s="2">
-        <v>14088.8</v>
+        <v>113032</v>
       </c>
       <c r="L46" s="4">
         <f t="shared" si="11"/>
-        <v>-97911.199999999983</v>
+        <v>1032.0000000000146</v>
       </c>
       <c r="M46" s="9">
         <f t="shared" si="12"/>
-        <v>-45.903047351148608</v>
+        <v>0.48382559774965522</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -5444,27 +5444,27 @@
       </c>
       <c r="F47" s="4"/>
       <c r="G47" s="2">
-        <v>61.738100000000003</v>
+        <v>353.49200000000002</v>
       </c>
       <c r="H47" s="4">
         <f t="shared" si="10"/>
-        <v>-292.81758619077607</v>
+        <v>-1.0636861907760817</v>
       </c>
       <c r="I47" s="9">
         <f t="shared" si="8"/>
-        <v>-46.648866281224223</v>
+        <v>-0.16945619805215525</v>
       </c>
       <c r="J47" s="2"/>
       <c r="K47" s="2">
-        <v>14491.5</v>
+        <v>116272</v>
       </c>
       <c r="L47" s="4">
         <f t="shared" si="11"/>
-        <v>-100708.49999999999</v>
+        <v>1072.0000000000146</v>
       </c>
       <c r="M47" s="9">
         <f t="shared" si="12"/>
-        <v>-46.516628175519628</v>
+        <v>0.49515011547344784</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
@@ -5490,27 +5490,27 @@
       </c>
       <c r="F48" s="4"/>
       <c r="G48" s="2">
-        <v>62.897300000000001</v>
+        <v>362.74299999999999</v>
       </c>
       <c r="H48" s="4">
         <f t="shared" si="10"/>
-        <v>-300.970044838219</v>
+        <v>-1.124344838218974</v>
       </c>
       <c r="I48" s="9">
         <f t="shared" si="8"/>
-        <v>-47.246758236175708</v>
+        <v>-0.17650144808922275</v>
       </c>
       <c r="J48" s="2"/>
       <c r="K48" s="2">
-        <v>14894.2</v>
+        <v>119513</v>
       </c>
       <c r="L48" s="4">
         <f t="shared" si="11"/>
-        <v>-103505.79999999999</v>
+        <v>1113.0000000000146</v>
       </c>
       <c r="M48" s="9">
         <f t="shared" si="12"/>
-        <v>-47.11233500227582</v>
+        <v>0.50659990896677942</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
@@ -5536,27 +5536,27 @@
       </c>
       <c r="F49" s="4"/>
       <c r="G49" s="2">
-        <v>64.0565</v>
+        <v>371.99200000000002</v>
       </c>
       <c r="H49" s="4">
         <f t="shared" si="10"/>
-        <v>-309.12350255249476</v>
+        <v>-1.1880025524947655</v>
       </c>
       <c r="I49" s="9">
         <f t="shared" si="8"/>
-        <v>-47.827503184395006</v>
+        <v>-0.18380742775410247</v>
       </c>
       <c r="J49" s="2"/>
       <c r="K49" s="2">
-        <v>15297</v>
+        <v>122755</v>
       </c>
       <c r="L49" s="4">
         <f t="shared" si="11"/>
-        <v>-106302.99999999999</v>
+        <v>1155.0000000000146</v>
       </c>
       <c r="M49" s="9">
         <f t="shared" si="12"/>
-        <v>-47.690892777030051</v>
+        <v>0.51816958277255032</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
@@ -5582,27 +5582,27 @@
       </c>
       <c r="F50" s="4"/>
       <c r="G50" s="2">
-        <v>65.215699999999998</v>
+        <v>381.24099999999999</v>
       </c>
       <c r="H50" s="4">
         <f t="shared" si="10"/>
-        <v>-317.27795949436961</v>
+        <v>-1.2526594943695954</v>
       </c>
       <c r="I50" s="9">
         <f t="shared" si="8"/>
-        <v>-48.391829143753704</v>
+        <v>-0.19105797428677077</v>
       </c>
       <c r="J50" s="2"/>
       <c r="K50" s="2">
-        <v>15699.7</v>
+        <v>125997</v>
       </c>
       <c r="L50" s="4">
         <f t="shared" si="11"/>
-        <v>-109100.29999999997</v>
+        <v>1197.0000000000291</v>
       </c>
       <c r="M50" s="9">
         <f t="shared" si="12"/>
-        <v>-48.253118089340994</v>
+        <v>0.52941176470589524</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
@@ -5628,27 +5628,27 @@
       </c>
       <c r="F51" s="4"/>
       <c r="G51" s="2">
-        <v>66.374799999999993</v>
+        <v>390.48899999999998</v>
       </c>
       <c r="H51" s="4">
         <f t="shared" si="10"/>
-        <v>-325.43351582464419</v>
+        <v>-1.3193158246442067</v>
       </c>
       <c r="I51" s="9">
         <f t="shared" si="8"/>
-        <v>-48.940438532761213</v>
+        <v>-0.19840579375386336</v>
       </c>
       <c r="J51" s="2"/>
       <c r="K51" s="2">
-        <v>16102.4</v>
+        <v>129240</v>
       </c>
       <c r="L51" s="4">
         <f t="shared" si="11"/>
-        <v>-111897.59999999998</v>
+        <v>1240.0000000000291</v>
       </c>
       <c r="M51" s="9">
         <f t="shared" si="12"/>
-        <v>-48.799651112080241</v>
+        <v>0.54077627562146935</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
@@ -5674,27 +5674,27 @@
       </c>
       <c r="F52" s="4"/>
       <c r="G52" s="2">
-        <v>67.533900000000003</v>
+        <v>399.73599999999999</v>
       </c>
       <c r="H52" s="4">
         <f t="shared" si="10"/>
-        <v>-333.59007170415373</v>
+        <v>-1.387971704153756</v>
       </c>
       <c r="I52" s="9">
         <f t="shared" si="8"/>
-        <v>-49.473965435895636</v>
+        <v>-0.20584684600027039</v>
       </c>
       <c r="J52" s="2"/>
       <c r="K52" s="2">
-        <v>16505.2</v>
+        <v>132483</v>
       </c>
       <c r="L52" s="4">
         <f t="shared" si="11"/>
-        <v>-114694.79999999997</v>
+        <v>1283.0000000000291</v>
       </c>
       <c r="M52" s="9">
         <f t="shared" si="12"/>
-        <v>-49.331096774193547</v>
+        <v>0.5518279569892599</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
@@ -5720,27 +5720,27 @@
       </c>
       <c r="F53" s="4"/>
       <c r="G53" s="2">
-        <v>68.693100000000001</v>
+        <v>408.983</v>
       </c>
       <c r="H53" s="4">
         <f t="shared" si="10"/>
-        <v>-341.7475272937682</v>
+        <v>-1.457627293768212</v>
       </c>
       <c r="I53" s="9">
         <f t="shared" si="8"/>
-        <v>-49.993009507268248</v>
+        <v>-0.21323102388614334</v>
       </c>
       <c r="J53" s="2"/>
       <c r="K53" s="2">
-        <v>16908</v>
+        <v>135727</v>
       </c>
       <c r="L53" s="4">
         <f t="shared" si="11"/>
-        <v>-117491.99999999997</v>
+        <v>1327.0000000000291</v>
       </c>
       <c r="M53" s="9">
         <f t="shared" si="12"/>
-        <v>-49.848112006788284</v>
+        <v>0.56300381841324965</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
@@ -5766,27 +5766,27 @@
       </c>
       <c r="F54" s="4"/>
       <c r="G54" s="2">
-        <v>69.852199999999996</v>
+        <v>418.22800000000001</v>
       </c>
       <c r="H54" s="4">
         <f t="shared" si="10"/>
-        <v>-349.90608275439178</v>
+        <v>-1.5302827543917488</v>
       </c>
       <c r="I54" s="9">
         <f t="shared" si="8"/>
-        <v>-50.498181572238401</v>
+        <v>-0.22084925126146498</v>
       </c>
       <c r="J54" s="2"/>
       <c r="K54" s="2">
-        <v>17310.7</v>
+        <v>138971</v>
       </c>
       <c r="L54" s="4">
         <f t="shared" si="11"/>
-        <v>-120289.29999999997</v>
+        <v>1371.0000000000291</v>
       </c>
       <c r="M54" s="9">
         <f t="shared" si="12"/>
-        <v>-50.351318543323565</v>
+        <v>0.57388028463793606</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
@@ -5812,27 +5812,27 @@
       </c>
       <c r="F55" s="4"/>
       <c r="G55" s="2">
-        <v>71.011300000000006</v>
+        <v>427.47300000000001</v>
       </c>
       <c r="H55" s="4">
         <f t="shared" si="10"/>
-        <v>-358.06563824696309</v>
+        <v>-1.6039382469630823</v>
       </c>
       <c r="I55" s="9">
         <f t="shared" si="8"/>
-        <v>-50.990017435223564</v>
+        <v>-0.22840739362223103</v>
       </c>
       <c r="J55" s="2"/>
       <c r="K55" s="2">
-        <v>17713.5</v>
+        <v>142216</v>
       </c>
       <c r="L55" s="4">
         <f t="shared" si="11"/>
-        <v>-123086.49999999997</v>
+        <v>1416.0000000000291</v>
       </c>
       <c r="M55" s="9">
         <f t="shared" si="12"/>
-        <v>-50.841181330028903</v>
+        <v>0.58488228004957843</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
@@ -5858,27 +5858,27 @@
       </c>
       <c r="F56" s="4"/>
       <c r="G56" s="2">
-        <v>72.170400000000001</v>
+        <v>436.71800000000002</v>
       </c>
       <c r="H56" s="4">
         <f t="shared" si="10"/>
-        <v>-366.22619393245566</v>
+        <v>-1.6785939324556125</v>
       </c>
       <c r="I56" s="9">
         <f t="shared" si="8"/>
-        <v>-51.469038999745408</v>
+        <v>-0.23590780235186606</v>
       </c>
       <c r="J56" s="2"/>
       <c r="K56" s="2">
-        <v>18116.3</v>
+        <v>145462</v>
       </c>
       <c r="L56" s="4">
         <f t="shared" si="11"/>
-        <v>-125883.69999999997</v>
+        <v>1462.0000000000291</v>
       </c>
       <c r="M56" s="9">
         <f t="shared" si="12"/>
-        <v>-51.31826335099877</v>
+        <v>0.59600489196902939</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
@@ -5904,27 +5904,27 @@
       </c>
       <c r="F57" s="4"/>
       <c r="G57" s="2">
-        <v>73.329499999999996</v>
+        <v>445.96100000000001</v>
       </c>
       <c r="H57" s="4">
         <f t="shared" si="10"/>
-        <v>-374.3877499718771</v>
+        <v>-1.7562499718770823</v>
       </c>
       <c r="I57" s="9">
         <f t="shared" si="8"/>
-        <v>-51.935741287523186</v>
+        <v>-0.24363015131365703</v>
       </c>
       <c r="J57" s="2"/>
       <c r="K57" s="2">
-        <v>18519.099999999999</v>
+        <v>148708</v>
       </c>
       <c r="L57" s="4">
         <f t="shared" si="11"/>
-        <v>-128680.89999999997</v>
+        <v>1508.0000000000291</v>
       </c>
       <c r="M57" s="9">
         <f t="shared" si="12"/>
-        <v>-51.783058350100596</v>
+        <v>0.60684104627767776</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -5950,27 +5950,27 @@
       </c>
       <c r="F58" s="4"/>
       <c r="G58" s="2">
-        <v>74.488500000000002</v>
+        <v>455.20400000000001</v>
       </c>
       <c r="H58" s="4">
         <f t="shared" si="10"/>
-        <v>-382.55040652627025</v>
+        <v>-1.8349065262702311</v>
       </c>
       <c r="I58" s="9">
         <f t="shared" si="8"/>
-        <v>-52.390607842315553</v>
+        <v>-0.25129203003089118</v>
       </c>
       <c r="J58" s="2"/>
       <c r="K58" s="2">
-        <v>18921.900000000001</v>
+        <v>151955</v>
       </c>
       <c r="L58" s="4">
         <f t="shared" si="11"/>
-        <v>-131478.09999999998</v>
+        <v>1555.0000000000291</v>
       </c>
       <c r="M58" s="9">
         <f t="shared" si="12"/>
-        <v>-52.236034962256653</v>
+        <v>0.61779896702424686</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
@@ -5996,27 +5996,27 @@
       </c>
       <c r="F59" s="4"/>
       <c r="G59" s="2">
-        <v>75.647599999999997</v>
+        <v>464.44600000000003</v>
       </c>
       <c r="H59" s="4">
         <f t="shared" si="10"/>
-        <v>-390.71396375671179</v>
+        <v>-1.9155637567117765</v>
       </c>
       <c r="I59" s="9">
         <f t="shared" si="8"/>
-        <v>-52.834057356978782</v>
+        <v>-0.25903094023043138</v>
       </c>
       <c r="J59" s="2"/>
       <c r="K59" s="2">
-        <v>19324.7</v>
+        <v>155203</v>
       </c>
       <c r="L59" s="4">
         <f t="shared" si="11"/>
-        <v>-134275.29999999996</v>
+        <v>1603.0000000000291</v>
       </c>
       <c r="M59" s="9">
         <f t="shared" si="12"/>
-        <v>-52.677638289525298</v>
+        <v>0.62887406826207504</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
@@ -6042,27 +6042,27 @@
       </c>
       <c r="F60" s="4"/>
       <c r="G60" s="2">
-        <v>76.806600000000003</v>
+        <v>473.68799999999999</v>
       </c>
       <c r="H60" s="4">
         <f t="shared" si="10"/>
-        <v>-398.87862182431331</v>
+        <v>-1.9972218243133284</v>
       </c>
       <c r="I60" s="9">
         <f t="shared" si="8"/>
-        <v>-53.266541182793823</v>
+        <v>-0.26671045459743387</v>
       </c>
       <c r="J60" s="2"/>
       <c r="K60" s="2">
-        <v>19727.599999999999</v>
+        <v>158451</v>
       </c>
       <c r="L60" s="4">
         <f t="shared" si="11"/>
-        <v>-137072.39999999997</v>
+        <v>1651.0000000000291</v>
       </c>
       <c r="M60" s="9">
         <f t="shared" si="12"/>
-        <v>-53.108252615265393</v>
+        <v>0.63967454475010821</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
@@ -6088,27 +6088,27 @@
       </c>
       <c r="F61" s="4"/>
       <c r="G61" s="2">
-        <v>77.965699999999998</v>
+        <v>482.92899999999997</v>
       </c>
       <c r="H61" s="4">
         <f t="shared" si="10"/>
-        <v>-407.04418089022101</v>
+        <v>-2.0808808902210103</v>
       </c>
       <c r="I61" s="9">
         <f t="shared" si="8"/>
-        <v>-53.688435796981935</v>
+        <v>-0.27446465352105792</v>
       </c>
       <c r="J61" s="2"/>
       <c r="K61" s="2">
-        <v>20130.400000000001</v>
+        <v>161699</v>
       </c>
       <c r="L61" s="4">
         <f t="shared" si="11"/>
-        <v>-139869.59999999998</v>
+        <v>1699.0000000000291</v>
       </c>
       <c r="M61" s="9">
         <f t="shared" si="12"/>
-        <v>-53.528358208955218</v>
+        <v>0.65021048603139275</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
@@ -6134,27 +6134,27 @@
       </c>
       <c r="F62" s="4"/>
       <c r="G62" s="2">
-        <v>79.124700000000004</v>
+        <v>492.16899999999998</v>
       </c>
       <c r="H62" s="4">
         <f t="shared" si="10"/>
-        <v>-415.21084111561566</v>
+        <v>-2.1665411156157006</v>
       </c>
       <c r="I62" s="9">
         <f t="shared" si="8"/>
-        <v>-54.10015158227813</v>
+        <v>-0.28229080543542495</v>
       </c>
       <c r="J62" s="2"/>
       <c r="K62" s="2">
-        <v>20533.2</v>
+        <v>164949</v>
       </c>
       <c r="L62" s="4">
         <f t="shared" si="11"/>
-        <v>-142666.79999999996</v>
+        <v>1749.0000000000291</v>
       </c>
       <c r="M62" s="9">
         <f t="shared" si="12"/>
-        <v>-53.938298676748566</v>
+        <v>0.66124763705105072</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
@@ -6180,27 +6180,27 @@
       </c>
       <c r="F63" s="4"/>
       <c r="G63" s="2">
-        <v>80.283699999999996</v>
+        <v>501.40800000000002</v>
       </c>
       <c r="H63" s="4">
         <f t="shared" si="10"/>
-        <v>-423.37850266171228</v>
+        <v>-2.2542026617122701</v>
       </c>
       <c r="I63" s="9">
         <f t="shared" si="8"/>
-        <v>-54.502040674827811</v>
+        <v>-0.2901863093793256</v>
       </c>
       <c r="J63" s="2"/>
       <c r="K63" s="2">
-        <v>20936.099999999999</v>
+        <v>168199</v>
       </c>
       <c r="L63" s="4">
         <f t="shared" si="11"/>
-        <v>-145463.89999999997</v>
+        <v>1799.0000000000291</v>
       </c>
       <c r="M63" s="9">
         <f t="shared" si="12"/>
-        <v>-54.338401195367936</v>
+        <v>0.67202091893912186</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
@@ -6226,27 +6226,27 @@
       </c>
       <c r="F64" s="4"/>
       <c r="G64" s="2">
-        <v>81.442700000000002</v>
+        <v>510.64600000000002</v>
       </c>
       <c r="H64" s="4">
         <f t="shared" si="10"/>
-        <v>-431.54716568976136</v>
+        <v>-2.3438656897613441</v>
       </c>
       <c r="I64" s="9">
         <f t="shared" si="8"/>
-        <v>-54.8944512960325</v>
+        <v>-0.29814868728287047</v>
       </c>
       <c r="J64" s="2"/>
       <c r="K64" s="2">
-        <v>21339</v>
+        <v>171449</v>
       </c>
       <c r="L64" s="4">
         <f t="shared" si="11"/>
-        <v>-148260.99999999997</v>
+        <v>1849.0000000000291</v>
       </c>
       <c r="M64" s="9">
         <f t="shared" si="12"/>
-        <v>-54.72905131044665</v>
+        <v>0.68253968253969333</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
@@ -6272,27 +6272,27 @@
       </c>
       <c r="F65" s="4"/>
       <c r="G65" s="2">
-        <v>82.601699999999994</v>
+        <v>519.88400000000001</v>
       </c>
       <c r="H65" s="4">
         <f t="shared" si="10"/>
-        <v>-439.7168303610469</v>
+        <v>-2.4345303610468818</v>
       </c>
       <c r="I65" s="9">
         <f t="shared" si="8"/>
-        <v>-55.277715406474783</v>
+        <v>-0.30604986471833129</v>
       </c>
       <c r="J65" s="2"/>
       <c r="K65" s="2">
-        <v>21741.8</v>
+        <v>174700</v>
       </c>
       <c r="L65" s="4">
         <f t="shared" si="11"/>
-        <v>-151058.19999999998</v>
+        <v>1900.0000000000291</v>
       </c>
       <c r="M65" s="9">
         <f t="shared" si="12"/>
-        <v>-55.110616563298066</v>
+        <v>0.69317767238235284</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
@@ -6318,27 +6318,27 @@
       </c>
       <c r="F66" s="4"/>
       <c r="G66" s="2">
-        <v>83.7607</v>
+        <v>529.12099999999998</v>
       </c>
       <c r="H66" s="4">
         <f t="shared" si="10"/>
-        <v>-447.88749683688849</v>
+        <v>-2.5271968368884927</v>
       </c>
       <c r="I66" s="9">
         <f t="shared" si="8"/>
-        <v>-55.652149644125458</v>
+        <v>-0.31401621509853972</v>
       </c>
       <c r="J66" s="2"/>
       <c r="K66" s="2">
-        <v>22144.7</v>
+        <v>177952</v>
       </c>
       <c r="L66" s="4">
         <f t="shared" si="11"/>
-        <v>-153855.29999999996</v>
+        <v>1952.0000000000291</v>
       </c>
       <c r="M66" s="9">
         <f t="shared" si="12"/>
-        <v>-55.483339343671098</v>
+        <v>0.7039307609087736</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
@@ -6364,27 +6364,27 @@
       </c>
       <c r="F67" s="4"/>
       <c r="G67" s="2">
-        <v>84.919700000000006</v>
+        <v>538.35799999999995</v>
       </c>
       <c r="H67" s="4">
         <f t="shared" si="10"/>
-        <v>-456.05916527863974</v>
+        <v>-2.6208652786398261</v>
       </c>
       <c r="I67" s="9">
         <f t="shared" si="8"/>
-        <v>-56.018056198333063</v>
+        <v>-0.32192265750739862</v>
       </c>
       <c r="J67" s="2"/>
       <c r="K67" s="2">
-        <v>22547.599999999999</v>
+        <v>181204</v>
       </c>
       <c r="L67" s="4">
         <f t="shared" si="11"/>
-        <v>-156652.39999999997</v>
+        <v>2004.0000000000291</v>
       </c>
       <c r="M67" s="9">
         <f t="shared" si="12"/>
-        <v>-55.847557932263804</v>
+        <v>0.71443850267380715</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
@@ -6410,27 +6410,27 @@
       </c>
       <c r="F68" s="4"/>
       <c r="G68" s="2">
-        <v>86.078599999999994</v>
+        <v>547.59299999999996</v>
       </c>
       <c r="H68" s="4">
         <f t="shared" si="10"/>
-        <v>-464.23193584768904</v>
+        <v>-2.7175358476890779</v>
       </c>
       <c r="I68" s="9">
         <f t="shared" si="8"/>
-        <v>-56.375735768539059</v>
+        <v>-0.33001409653367114</v>
       </c>
       <c r="J68" s="2"/>
       <c r="K68" s="2">
-        <v>22950.5</v>
+        <v>184457</v>
       </c>
       <c r="L68" s="4">
         <f t="shared" si="11"/>
-        <v>-159449.49999999997</v>
+        <v>2057.0000000000291</v>
       </c>
       <c r="M68" s="9">
         <f t="shared" si="12"/>
-        <v>-56.203560098695796</v>
+        <v>0.72506168487840295</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
@@ -6456,27 +6456,27 @@
       </c>
       <c r="F69" s="4"/>
       <c r="G69" s="2">
-        <v>87.2376</v>
+        <v>556.82799999999997</v>
       </c>
       <c r="H69" s="4">
         <f t="shared" si="10"/>
-        <v>-472.40560870545988</v>
+        <v>-2.8152087054598951</v>
       </c>
       <c r="I69" s="9">
         <f t="shared" si="8"/>
-        <v>-56.725439613009513</v>
+        <v>-0.33804414781864184</v>
       </c>
       <c r="J69" s="2"/>
       <c r="K69" s="2">
-        <v>23353.4</v>
+        <v>187710</v>
       </c>
       <c r="L69" s="4">
         <f t="shared" si="11"/>
-        <v>-162246.59999999998</v>
+        <v>2110.0000000000291</v>
       </c>
       <c r="M69" s="9">
         <f t="shared" si="12"/>
-        <v>-56.55162077378877</v>
+        <v>0.73544789125131715</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
@@ -6502,27 +6502,27 @@
       </c>
       <c r="F70" s="4"/>
       <c r="G70" s="2">
-        <v>88.396500000000003</v>
+        <v>566.06200000000001</v>
       </c>
       <c r="H70" s="4">
         <f t="shared" si="10"/>
-        <v>-480.58038401340974</v>
+        <v>-2.9148840134097327</v>
       </c>
       <c r="I70" s="9">
         <f t="shared" si="8"/>
-        <v>-57.067455408032927</v>
+        <v>-0.34613358969351193</v>
       </c>
       <c r="J70" s="2"/>
       <c r="K70" s="2">
-        <v>23756.400000000001</v>
+        <v>190964</v>
       </c>
       <c r="L70" s="4">
         <f t="shared" si="11"/>
-        <v>-165043.59999999998</v>
+        <v>2164.0000000000291</v>
       </c>
       <c r="M70" s="9">
         <f t="shared" si="12"/>
-        <v>-56.891968286797642</v>
+        <v>0.74594967252672495</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
@@ -6548,27 +6548,27 @@
       </c>
       <c r="F71" s="4"/>
       <c r="G71" s="2">
-        <v>89.555400000000006</v>
+        <v>575.29600000000005</v>
       </c>
       <c r="H71" s="4">
         <f t="shared" si="10"/>
-        <v>-488.75616193303102</v>
+        <v>-3.0155619330309946</v>
       </c>
       <c r="I71" s="9">
         <f t="shared" si="8"/>
-        <v>-57.402023037121261</v>
+        <v>-0.3541630142627829</v>
       </c>
       <c r="J71" s="2"/>
       <c r="K71" s="2">
-        <v>24159.3</v>
+        <v>194219</v>
       </c>
       <c r="L71" s="4">
         <f t="shared" si="11"/>
-        <v>-167840.69999999998</v>
+        <v>2219.0000000000291</v>
       </c>
       <c r="M71" s="9">
         <f t="shared" si="12"/>
-        <v>-57.22492328673713</v>
+        <v>0.75656324582339896</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
@@ -6594,27 +6594,27 @@
       </c>
       <c r="F72" s="4"/>
       <c r="G72" s="2">
-        <v>90.714299999999994</v>
+        <v>584.52800000000002</v>
       </c>
       <c r="H72" s="4">
         <f t="shared" si="10"/>
-        <v>-496.93294262585118</v>
+        <v>-3.1192426258511432</v>
       </c>
       <c r="I72" s="9">
         <f t="shared" si="8"/>
-        <v>-57.729383647880127</v>
+        <v>-0.36236670744157273</v>
       </c>
       <c r="J72" s="2"/>
       <c r="K72" s="2">
-        <v>24562.2</v>
+        <v>197474</v>
       </c>
       <c r="L72" s="4">
         <f t="shared" si="11"/>
-        <v>-170637.79999999996</v>
+        <v>2274.0000000000291</v>
       </c>
       <c r="M72" s="9">
         <f t="shared" si="12"/>
-        <v>-57.550691399662725</v>
+        <v>0.76694772344014472</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
@@ -6640,27 +6640,27 @@
       </c>
       <c r="F73" s="4"/>
       <c r="G73" s="2">
-        <v>91.873199999999997</v>
+        <v>593.76</v>
       </c>
       <c r="H73" s="4">
         <f t="shared" si="10"/>
-        <v>-505.11072625343172</v>
+        <v>-3.2239262534317277</v>
       </c>
       <c r="I73" s="9">
         <f t="shared" si="8"/>
-        <v>-58.049768088954522</v>
+        <v>-0.3705092004989517</v>
       </c>
       <c r="J73" s="2"/>
       <c r="K73" s="2">
-        <v>24965.200000000001</v>
+        <v>200730</v>
       </c>
       <c r="L73" s="4">
         <f t="shared" si="11"/>
-        <v>-173434.79999999996</v>
+        <v>2330.0000000000291</v>
       </c>
       <c r="M73" s="9">
         <f t="shared" si="12"/>
-        <v>-57.869469469469458</v>
+        <v>0.77744411077745379</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
@@ -6686,27 +6686,27 @@
       </c>
       <c r="F74" s="4"/>
       <c r="G74" s="2">
-        <v>93.0321</v>
+        <v>602.99099999999999</v>
       </c>
       <c r="H74" s="4">
         <f t="shared" si="10"/>
-        <v>-513.28951297736933</v>
+        <v>-3.3306129773693556</v>
       </c>
       <c r="I74" s="9">
         <f t="shared" si="8"/>
-        <v>-58.363397454032139</v>
+        <v>-0.37870613766530514</v>
       </c>
       <c r="J74" s="2"/>
       <c r="K74" s="2">
-        <v>25368.1</v>
+        <v>203987</v>
       </c>
       <c r="L74" s="4">
         <f t="shared" si="11"/>
-        <v>-176231.89999999997</v>
+        <v>2387.0000000000291</v>
       </c>
       <c r="M74" s="9">
         <f t="shared" si="12"/>
-        <v>-58.181545064377673</v>
+        <v>0.78804886101024407</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
@@ -6732,27 +6732,27 @@
       </c>
       <c r="F75" s="4"/>
       <c r="G75" s="2">
-        <v>94.191000000000003</v>
+        <v>612.22199999999998</v>
       </c>
       <c r="H75" s="4">
         <f t="shared" ref="H75:H101" si="18">G75-E75</f>
-        <v>-521.46930295929542</v>
+        <v>-3.4383029592954699</v>
       </c>
       <c r="I75" s="9">
         <f t="shared" si="8"/>
-        <v>-58.670483591725088</v>
+        <v>-0.38684328341465374</v>
       </c>
       <c r="J75" s="2"/>
       <c r="K75" s="2">
-        <v>25771.1</v>
+        <v>207244</v>
       </c>
       <c r="L75" s="4">
         <f t="shared" ref="L75:L101" si="19">K75-C75</f>
-        <v>-179028.89999999997</v>
+        <v>2444.0000000000291</v>
       </c>
       <c r="M75" s="9">
         <f t="shared" ref="M75:M101" si="20">L75/(C75+P0)*100</f>
-        <v>-58.487063051290413</v>
+        <v>0.79843188500490991</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
@@ -6778,27 +6778,27 @@
       </c>
       <c r="F76" s="4"/>
       <c r="G76" s="2">
-        <v>95.349900000000005</v>
+        <v>621.452</v>
       </c>
       <c r="H76" s="4">
         <f t="shared" si="18"/>
-        <v>-529.65009636087564</v>
+        <v>-3.5479963608756862</v>
       </c>
       <c r="I76" s="9">
         <f t="shared" si="8"/>
-        <v>-58.971229583801367</v>
+        <v>-0.39503383346339233</v>
       </c>
       <c r="J76" s="2"/>
       <c r="K76" s="2">
-        <v>26174.1</v>
+        <v>210501</v>
       </c>
       <c r="L76" s="4">
         <f t="shared" si="19"/>
-        <v>-181825.89999999997</v>
+        <v>2501.0000000000291</v>
       </c>
       <c r="M76" s="9">
         <f t="shared" si="20"/>
-        <v>-58.78625929518266</v>
+        <v>0.80860006466214973</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
@@ -6824,27 +6824,27 @@
       </c>
       <c r="F77" s="4"/>
       <c r="G77" s="2">
-        <v>96.508700000000005</v>
+        <v>630.68100000000004</v>
       </c>
       <c r="H77" s="4">
         <f t="shared" si="18"/>
-        <v>-537.83199334381106</v>
+        <v>-3.659693343811</v>
       </c>
       <c r="I77" s="9">
         <f t="shared" ref="I77:I101" si="24">H77/(E77+273.15)*100</f>
-        <v>-59.265841213431436</v>
+        <v>-0.40327612951337372</v>
       </c>
       <c r="J77" s="2"/>
       <c r="K77" s="2">
-        <v>26577.1</v>
+        <v>213759</v>
       </c>
       <c r="L77" s="4">
         <f t="shared" si="19"/>
-        <v>-184622.89999999997</v>
+        <v>2559.0000000000291</v>
       </c>
       <c r="M77" s="9">
         <f t="shared" si="20"/>
-        <v>-59.07932799999999</v>
+        <v>0.81888000000000938</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
@@ -6870,27 +6870,27 @@
       </c>
       <c r="F78" s="4"/>
       <c r="G78" s="2">
-        <v>97.667500000000004</v>
+        <v>639.90899999999999</v>
       </c>
       <c r="H78" s="4">
         <f t="shared" si="18"/>
-        <v>-546.01489406983694</v>
+        <v>-3.7733940698369679</v>
       </c>
       <c r="I78" s="9">
         <f t="shared" si="24"/>
-        <v>-59.554494103994969</v>
+        <v>-0.41156858049995348</v>
       </c>
       <c r="J78" s="2"/>
       <c r="K78" s="2">
-        <v>26980.1</v>
+        <v>217018</v>
       </c>
       <c r="L78" s="4">
         <f t="shared" si="19"/>
-        <v>-187419.89999999997</v>
+        <v>2618.0000000000291</v>
       </c>
       <c r="M78" s="9">
         <f t="shared" si="20"/>
-        <v>-59.366455495723777</v>
+        <v>0.82926829268293611</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
@@ -6916,27 +6916,27 @@
       </c>
       <c r="F79" s="4"/>
       <c r="G79" s="2">
-        <v>98.826400000000007</v>
+        <v>649.13699999999994</v>
       </c>
       <c r="H79" s="4">
         <f t="shared" si="18"/>
-        <v>-554.1986987007233</v>
+        <v>-3.8880987007233898</v>
       </c>
       <c r="I79" s="9">
         <f t="shared" si="24"/>
-        <v>-59.837356832220614</v>
+        <v>-0.41980168827447156</v>
       </c>
       <c r="J79" s="2"/>
       <c r="K79" s="2">
-        <v>27383.1</v>
+        <v>220278</v>
       </c>
       <c r="L79" s="4">
         <f t="shared" si="19"/>
-        <v>-190216.89999999997</v>
+        <v>2678.0000000000291</v>
       </c>
       <c r="M79" s="9">
         <f t="shared" si="20"/>
-        <v>-59.647820633427393</v>
+        <v>0.83976168077768232</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
@@ -6962,27 +6962,27 @@
       </c>
       <c r="F80" s="4"/>
       <c r="G80" s="2">
-        <v>99.985200000000006</v>
+        <v>658.36300000000006</v>
       </c>
       <c r="H80" s="4">
         <f t="shared" si="18"/>
-        <v>-562.38360739827533</v>
+        <v>-4.0058073982752376</v>
       </c>
       <c r="I80" s="9">
         <f t="shared" si="24"/>
-        <v>-60.114623345979787</v>
+        <v>-0.42819100659404047</v>
       </c>
       <c r="J80" s="2"/>
       <c r="K80" s="2">
-        <v>27786.1</v>
+        <v>223538</v>
       </c>
       <c r="L80" s="4">
         <f t="shared" si="19"/>
-        <v>-193013.89999999997</v>
+        <v>2738.0000000000291</v>
       </c>
       <c r="M80" s="9">
         <f t="shared" si="20"/>
-        <v>-59.923595156783591</v>
+        <v>0.85004656938839762</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
@@ -7008,27 +7008,27 @@
       </c>
       <c r="F81" s="4"/>
       <c r="G81" s="2">
-        <v>101.14400000000001</v>
+        <v>667.59</v>
       </c>
       <c r="H81" s="4">
         <f t="shared" si="18"/>
-        <v>-570.56952032433253</v>
+        <v>-4.1235203243325032</v>
       </c>
       <c r="I81" s="9">
         <f t="shared" si="24"/>
-        <v>-60.386448206665833</v>
+        <v>-0.43641438531959298</v>
       </c>
       <c r="J81" s="2"/>
       <c r="K81" s="2">
-        <v>28189.1</v>
+        <v>226798</v>
       </c>
       <c r="L81" s="4">
         <f t="shared" si="19"/>
-        <v>-195810.89999999997</v>
+        <v>2798.0000000000291</v>
       </c>
       <c r="M81" s="9">
         <f t="shared" si="20"/>
-        <v>-60.193944051644621</v>
+        <v>0.86012911158931116</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
@@ -7054,27 +7054,27 @@
       </c>
       <c r="F82" s="4"/>
       <c r="G82" s="2">
-        <v>102.303</v>
+        <v>676.81500000000005</v>
       </c>
       <c r="H82" s="4">
         <f t="shared" si="18"/>
-        <v>-578.75623764076954</v>
+        <v>-4.2442376407694837</v>
       </c>
       <c r="I82" s="9">
         <f t="shared" si="24"/>
-        <v>-60.652969475721378</v>
+        <v>-0.44479108704324966</v>
       </c>
       <c r="J82" s="2"/>
       <c r="K82" s="2">
-        <v>28592.2</v>
+        <v>230060</v>
       </c>
       <c r="L82" s="4">
         <f t="shared" si="19"/>
-        <v>-198607.79999999996</v>
+        <v>2860.0000000000291</v>
       </c>
       <c r="M82" s="9">
         <f t="shared" si="20"/>
-        <v>-60.458995433789944</v>
+        <v>0.87062404870624932</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
@@ -7100,27 +7100,27 @@
       </c>
       <c r="F83" s="4"/>
       <c r="G83" s="2">
-        <v>103.462</v>
+        <v>686.04</v>
       </c>
       <c r="H83" s="4">
         <f t="shared" si="18"/>
-        <v>-586.9439595094957</v>
+        <v>-4.365959509495724</v>
       </c>
       <c r="I83" s="9">
         <f t="shared" si="24"/>
-        <v>-60.914361404425676</v>
+        <v>-0.45310907647940274</v>
       </c>
       <c r="J83" s="2"/>
       <c r="K83" s="2">
-        <v>28995.200000000001</v>
+        <v>233321</v>
       </c>
       <c r="L83" s="4">
         <f t="shared" si="19"/>
-        <v>-201404.79999999996</v>
+        <v>2921.0000000000291</v>
       </c>
       <c r="M83" s="9">
         <f t="shared" si="20"/>
-        <v>-60.71896291829966</v>
+        <v>0.88061501356648442</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
@@ -7146,27 +7146,27 @@
       </c>
       <c r="F84" s="4"/>
       <c r="G84" s="2">
-        <v>104.62</v>
+        <v>695.26400000000001</v>
       </c>
       <c r="H84" s="4">
         <f t="shared" si="18"/>
-        <v>-595.13368609245515</v>
+        <v>-4.4896860924551447</v>
       </c>
       <c r="I84" s="9">
         <f t="shared" si="24"/>
-        <v>-61.170873807944389</v>
+        <v>-0.46147282168159959</v>
       </c>
       <c r="J84" s="2"/>
       <c r="K84" s="2">
-        <v>29398.3</v>
+        <v>236584</v>
       </c>
       <c r="L84" s="4">
         <f t="shared" si="19"/>
-        <v>-204201.69999999998</v>
+        <v>2984.0000000000291</v>
       </c>
       <c r="M84" s="9">
         <f t="shared" si="20"/>
-        <v>-60.973932517169295</v>
+        <v>0.89101224246044464</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
@@ -7192,27 +7192,27 @@
       </c>
       <c r="F85" s="4"/>
       <c r="G85" s="2">
-        <v>105.779</v>
+        <v>704.48699999999997</v>
       </c>
       <c r="H85" s="4">
         <f t="shared" si="18"/>
-        <v>-603.32341755162633</v>
+        <v>-4.6154175516263649</v>
       </c>
       <c r="I85" s="9">
         <f t="shared" si="24"/>
-        <v>-61.422441601668666</v>
+        <v>-0.46988100707665431</v>
       </c>
       <c r="J85" s="2"/>
       <c r="K85" s="2">
-        <v>29801.3</v>
+        <v>239847</v>
       </c>
       <c r="L85" s="4">
         <f t="shared" si="19"/>
-        <v>-206998.69999999998</v>
+        <v>3047.0000000000291</v>
       </c>
       <c r="M85" s="9">
         <f t="shared" si="20"/>
-        <v>-61.224105294291618</v>
+        <v>0.90121265897664271</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
@@ -7238,27 +7238,27 @@
       </c>
       <c r="F86" s="4"/>
       <c r="G86" s="2">
-        <v>106.938</v>
+        <v>713.70899999999995</v>
       </c>
       <c r="H86" s="4">
         <f t="shared" si="18"/>
-        <v>-611.51415404902343</v>
+        <v>-4.7431540490234738</v>
       </c>
       <c r="I86" s="9">
         <f t="shared" si="24"/>
-        <v>-61.669304725894236</v>
+        <v>-0.47833236642898408</v>
       </c>
       <c r="J86" s="2"/>
       <c r="K86" s="2">
-        <v>30204.400000000001</v>
+        <v>243111</v>
       </c>
       <c r="L86" s="4">
         <f t="shared" si="19"/>
-        <v>-209795.59999999998</v>
+        <v>3111.0000000000291</v>
       </c>
       <c r="M86" s="9">
         <f t="shared" si="20"/>
-        <v>-61.469557573981824</v>
+        <v>0.9115147963668413</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
@@ -7284,27 +7284,27 @@
       </c>
       <c r="F87" s="4"/>
       <c r="G87" s="2">
-        <v>108.09699999999999</v>
+        <v>722.93100000000004</v>
       </c>
       <c r="H87" s="4">
         <f t="shared" si="18"/>
-        <v>-619.70589574669464</v>
+        <v>-4.8718957466945767</v>
       </c>
       <c r="I87" s="9">
         <f t="shared" si="24"/>
-        <v>-61.911594279809158</v>
+        <v>-0.48672577574794079</v>
       </c>
       <c r="J87" s="2"/>
       <c r="K87" s="2">
-        <v>30607.5</v>
+        <v>246375</v>
       </c>
       <c r="L87" s="4">
         <f t="shared" si="19"/>
-        <v>-212592.49999999997</v>
+        <v>3175.0000000000291</v>
       </c>
       <c r="M87" s="9">
         <f t="shared" si="20"/>
-        <v>-61.710449927431057</v>
+        <v>0.92162554426706222</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
@@ -7330,27 +7330,27 @@
       </c>
       <c r="F88" s="4"/>
       <c r="G88" s="2">
-        <v>109.255</v>
+        <v>732.15200000000004</v>
       </c>
       <c r="H88" s="4">
         <f t="shared" si="18"/>
-        <v>-627.89964280672348</v>
+        <v>-5.0026428067234292</v>
       </c>
       <c r="I88" s="9">
         <f t="shared" si="24"/>
-        <v>-62.149535516570317</v>
+        <v>-0.49516181503685924</v>
       </c>
       <c r="J88" s="2"/>
       <c r="K88" s="2">
-        <v>31010.6</v>
+        <v>249640</v>
       </c>
       <c r="L88" s="4">
         <f t="shared" si="19"/>
-        <v>-215389.39999999994</v>
+        <v>3240.0000000000582</v>
       </c>
       <c r="M88" s="9">
         <f t="shared" si="20"/>
-        <v>-61.946908254242153</v>
+        <v>0.93183779119932664</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
@@ -7376,27 +7376,27 @@
       </c>
       <c r="F89" s="4"/>
       <c r="G89" s="2">
-        <v>110.414</v>
+        <v>741.37199999999996</v>
       </c>
       <c r="H89" s="4">
         <f t="shared" si="18"/>
-        <v>-636.093395391228</v>
+        <v>-5.1353953912280303</v>
       </c>
       <c r="I89" s="9">
         <f t="shared" si="24"/>
-        <v>-62.383051235279673</v>
+        <v>-0.50363930222441555</v>
       </c>
       <c r="J89" s="2"/>
       <c r="K89" s="2">
-        <v>31413.7</v>
+        <v>252905</v>
       </c>
       <c r="L89" s="4">
         <f t="shared" si="19"/>
-        <v>-218186.29999999993</v>
+        <v>3305.0000000000582</v>
       </c>
       <c r="M89" s="9">
         <f t="shared" si="20"/>
-        <v>-62.179053861498993</v>
+        <v>0.9418637788543911</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
@@ -7422,27 +7422,27 @@
       </c>
       <c r="F90" s="4"/>
       <c r="G90" s="2">
-        <v>111.57299999999999</v>
+        <v>750.59199999999998</v>
       </c>
       <c r="H90" s="4">
         <f t="shared" si="18"/>
-        <v>-644.28815366236154</v>
+        <v>-5.269153662361532</v>
       </c>
       <c r="I90" s="9">
         <f t="shared" si="24"/>
-        <v>-62.61235860945439</v>
+        <v>-0.51205991729127975</v>
       </c>
       <c r="J90" s="2"/>
       <c r="K90" s="2">
-        <v>31816.799999999999</v>
+        <v>256171</v>
       </c>
       <c r="L90" s="4">
         <f t="shared" si="19"/>
-        <v>-220983.19999999995</v>
+        <v>3371.0000000000582</v>
       </c>
       <c r="M90" s="9">
         <f t="shared" si="20"/>
-        <v>-62.407003671279291</v>
+        <v>0.95199096300481756</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
@@ -7468,27 +7468,27 @@
       </c>
       <c r="F91" s="4"/>
       <c r="G91" s="2">
-        <v>112.73099999999999</v>
+        <v>759.81100000000004</v>
       </c>
       <c r="H91" s="4">
         <f t="shared" si="18"/>
-        <v>-652.48491778231153</v>
+        <v>-5.404917782311486</v>
       </c>
       <c r="I91" s="9">
         <f t="shared" si="24"/>
-        <v>-62.837667012015885</v>
+        <v>-0.52052149341101561</v>
       </c>
       <c r="J91" s="2"/>
       <c r="K91" s="2">
-        <v>32219.9</v>
+        <v>259438</v>
       </c>
       <c r="L91" s="4">
         <f t="shared" si="19"/>
-        <v>-223780.09999999995</v>
+        <v>3438.0000000000582</v>
       </c>
       <c r="M91" s="9">
         <f t="shared" si="20"/>
-        <v>-62.630870417016503</v>
+        <v>0.9622166246851549</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
@@ -7514,27 +7514,27 @@
       </c>
       <c r="F92" s="4"/>
       <c r="G92" s="2">
-        <v>113.89</v>
+        <v>769.029</v>
       </c>
       <c r="H92" s="4">
         <f t="shared" si="18"/>
-        <v>-660.68168791330095</v>
+        <v>-5.5426879133009379</v>
       </c>
       <c r="I92" s="9">
         <f t="shared" si="24"/>
-        <v>-63.058892025911028</v>
+        <v>-0.52902292443139687</v>
       </c>
       <c r="J92" s="2"/>
       <c r="K92" s="2">
-        <v>32623</v>
+        <v>262705</v>
       </c>
       <c r="L92" s="4">
         <f t="shared" si="19"/>
-        <v>-226576.99999999994</v>
+        <v>3505.0000000000582</v>
       </c>
       <c r="M92" s="9">
         <f t="shared" si="20"/>
-        <v>-62.850762829403592</v>
+        <v>0.97226074895979431</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
@@ -7560,27 +7560,27 @@
       </c>
       <c r="F93" s="4"/>
       <c r="G93" s="2">
-        <v>115.04900000000001</v>
+        <v>778.24599999999998</v>
       </c>
       <c r="H93" s="4">
         <f t="shared" si="18"/>
-        <v>-668.87946421758795</v>
+        <v>-5.682464217587949</v>
       </c>
       <c r="I93" s="9">
         <f t="shared" si="24"/>
-        <v>-63.276236046741232</v>
+        <v>-0.53756314312901154</v>
       </c>
       <c r="J93" s="2"/>
       <c r="K93" s="2">
-        <v>33026.199999999997</v>
+        <v>265973</v>
       </c>
       <c r="L93" s="4">
         <f t="shared" si="19"/>
-        <v>-229373.79999999993</v>
+        <v>3573.0000000000582</v>
       </c>
       <c r="M93" s="9">
         <f t="shared" si="20"/>
-        <v>-63.066758317294472</v>
+        <v>0.9824030794611105</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
@@ -7606,27 +7606,27 @@
       </c>
       <c r="F94" s="4"/>
       <c r="G94" s="2">
-        <v>116.20699999999999</v>
+        <v>787.46299999999997</v>
       </c>
       <c r="H94" s="4">
         <f t="shared" si="18"/>
-        <v>-677.07924685746434</v>
+        <v>-5.823246857464369</v>
       </c>
       <c r="I94" s="9">
         <f t="shared" si="24"/>
-        <v>-63.489894389154244</v>
+        <v>-0.54604734925543852</v>
       </c>
       <c r="J94" s="2"/>
       <c r="K94" s="2">
-        <v>33429.300000000003</v>
+        <v>269241</v>
       </c>
       <c r="L94" s="4">
         <f t="shared" si="19"/>
-        <v>-232170.69999999995</v>
+        <v>3641.0000000000582</v>
       </c>
       <c r="M94" s="9">
         <f t="shared" si="20"/>
-        <v>-63.279013355137636</v>
+        <v>0.99236849277733952</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
@@ -7652,27 +7652,27 @@
       </c>
       <c r="F95" s="4"/>
       <c r="G95" s="2">
-        <v>117.366</v>
+        <v>796.67899999999997</v>
       </c>
       <c r="H95" s="4">
         <f t="shared" si="18"/>
-        <v>-685.27903599525791</v>
+        <v>-5.9660359952579256</v>
       </c>
       <c r="I95" s="9">
         <f t="shared" si="24"/>
-        <v>-63.699776729428848</v>
+        <v>-0.55456995018930577</v>
       </c>
       <c r="J95" s="2"/>
       <c r="K95" s="2">
-        <v>33832.5</v>
+        <v>272510</v>
       </c>
       <c r="L95" s="4">
         <f t="shared" si="19"/>
-        <v>-234967.49999999994</v>
+        <v>3710.0000000000582</v>
       </c>
       <c r="M95" s="9">
         <f t="shared" si="20"/>
-        <v>-63.487570926776534</v>
+        <v>1.0024317751959089</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
@@ -7698,27 +7698,27 @@
       </c>
       <c r="F96" s="4"/>
       <c r="G96" s="2">
-        <v>118.52500000000001</v>
+        <v>805.89400000000001</v>
       </c>
       <c r="H96" s="4">
         <f t="shared" si="18"/>
-        <v>-693.47983179333073</v>
+        <v>-6.1108317933307035</v>
       </c>
       <c r="I96" s="9">
         <f t="shared" si="24"/>
-        <v>-63.906072338754051</v>
+        <v>-0.56312994369954761</v>
       </c>
       <c r="J96" s="2"/>
       <c r="K96" s="2">
-        <v>34235.599999999999</v>
+        <v>275780</v>
       </c>
       <c r="L96" s="4">
         <f t="shared" si="19"/>
-        <v>-237764.39999999994</v>
+        <v>3780.0000000000582</v>
       </c>
       <c r="M96" s="9">
         <f t="shared" si="20"/>
-        <v>-63.692579694615581</v>
+        <v>1.0125904098580389</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
@@ -7744,27 +7744,27 @@
       </c>
       <c r="F97" s="4"/>
       <c r="G97" s="2">
-        <v>119.68300000000001</v>
+        <v>815.10900000000004</v>
       </c>
       <c r="H97" s="4">
         <f t="shared" si="18"/>
-        <v>-701.68263441408033</v>
+        <v>-6.2566344140802812</v>
       </c>
       <c r="I97" s="9">
         <f t="shared" si="24"/>
-        <v>-64.10896403409599</v>
+        <v>-0.57163499701213527</v>
       </c>
       <c r="J97" s="2"/>
       <c r="K97" s="2">
-        <v>34638.800000000003</v>
+        <v>279050</v>
       </c>
       <c r="L97" s="4">
         <f t="shared" si="19"/>
-        <v>-240561.19999999995</v>
+        <v>3850.0000000000582</v>
       </c>
       <c r="M97" s="9">
         <f t="shared" si="20"/>
-        <v>-63.894077025232399</v>
+        <v>1.0225763612217953</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
@@ -7790,27 +7790,27 @@
       </c>
       <c r="F98" s="4"/>
       <c r="G98" s="2">
-        <v>120.842</v>
+        <v>824.322</v>
       </c>
       <c r="H98" s="4">
         <f t="shared" si="18"/>
-        <v>-709.88544401993909</v>
+        <v>-6.4054440199390683</v>
       </c>
       <c r="I98" s="9">
         <f t="shared" si="24"/>
-        <v>-64.30835668086327</v>
+        <v>-0.5802676786847516</v>
       </c>
       <c r="J98" s="2"/>
       <c r="K98" s="2">
-        <v>35042</v>
+        <v>282321</v>
       </c>
       <c r="L98" s="4">
         <f t="shared" si="19"/>
-        <v>-243357.99999999994</v>
+        <v>3921.0000000000582</v>
       </c>
       <c r="M98" s="9">
         <f t="shared" si="20"/>
-        <v>-64.092178035291013</v>
+        <v>1.032657361074548</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
@@ -7836,27 +7836,27 @@
       </c>
       <c r="F99" s="4"/>
       <c r="G99" s="2">
-        <v>122.001</v>
+        <v>833.53499999999997</v>
       </c>
       <c r="H99" s="4">
         <f t="shared" si="18"/>
-        <v>-718.08926077337367</v>
+        <v>-6.555260773373675</v>
       </c>
       <c r="I99" s="9">
         <f t="shared" si="24"/>
-        <v>-64.504427846915405</v>
+        <v>-0.5888451041844015</v>
       </c>
       <c r="J99" s="2"/>
       <c r="K99" s="2">
-        <v>35445.199999999997</v>
+        <v>285592</v>
       </c>
       <c r="L99" s="4">
         <f t="shared" si="19"/>
-        <v>-246154.79999999993</v>
+        <v>3992.0000000000582</v>
       </c>
       <c r="M99" s="9">
         <f t="shared" si="20"/>
-        <v>-64.286967876730202</v>
+        <v>1.0425698615826742</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
@@ -7882,27 +7882,27 @@
       </c>
       <c r="F100" s="4"/>
       <c r="G100" s="2">
-        <v>123.15900000000001</v>
+        <v>842.74800000000005</v>
       </c>
       <c r="H100" s="4">
         <f t="shared" si="18"/>
-        <v>-726.29508483688664</v>
+        <v>-6.7060848368865891</v>
       </c>
       <c r="I100" s="9">
         <f t="shared" si="24"/>
-        <v>-64.697349194343673</v>
+        <v>-0.5973686473678721</v>
       </c>
       <c r="J100" s="2"/>
       <c r="K100" s="2">
-        <v>35848.400000000001</v>
+        <v>288864</v>
       </c>
       <c r="L100" s="4">
         <f t="shared" si="19"/>
-        <v>-248951.59999999995</v>
+        <v>4064.0000000000582</v>
       </c>
       <c r="M100" s="9">
         <f t="shared" si="20"/>
-        <v>-64.478528878528877</v>
+        <v>1.0525770525770677</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
@@ -7928,27 +7928,27 @@
       </c>
       <c r="F101" s="4"/>
       <c r="G101" s="2">
-        <v>124.318</v>
+        <v>851.95899999999995</v>
       </c>
       <c r="H101" s="4">
         <f t="shared" si="18"/>
-        <v>-734.50091637301455</v>
+        <v>-6.8599163730145847</v>
       </c>
       <c r="I101" s="9">
         <f t="shared" si="24"/>
-        <v>-64.887021697243895</v>
+        <v>-0.60601632021793572</v>
       </c>
       <c r="J101" s="2"/>
       <c r="K101" s="2">
-        <v>36251.599999999999</v>
+        <v>292136</v>
       </c>
       <c r="L101" s="4">
         <f t="shared" si="19"/>
-        <v>-251748.39999999994</v>
+        <v>4136.0000000000582</v>
       </c>
       <c r="M101" s="9">
         <f t="shared" si="20"/>
-        <v>-64.666940662727967</v>
+        <v>1.0624197277164291</v>
       </c>
     </row>
   </sheetData>

</xml_diff>